<commit_message>
pcb: added C and rmd unneeded hardware
Signed-off-by: Dylan Turner <dylan.turner@tutanota.com>
</commit_message>
<xml_diff>
--- a/pcb/ps-ohk-bom.xlsx
+++ b/pcb/ps-ohk-bom.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ps-ohk" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ps-ohk" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -52,19 +52,19 @@
     <t xml:space="preserve">  WCH (Jiangsu Qin Heng) </t>
   </si>
   <si>
-    <t xml:space="preserve">R_I2C2,R_I2C1,R_SET1,R_SET4,R_ADDR1,R_SET3,R_SET2</t>
+    <t xml:space="preserve">R_I2C2,R_I2C1,R_ADDR1,R_PROG1</t>
   </si>
   <si>
     <t xml:space="preserve">R 0603</t>
   </si>
   <si>
-    <t xml:space="preserve">1k Ohm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welwyn Components / TT Electronics </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WCR0603-1K0FI </t>
+    <t xml:space="preserve">10k Ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity / Holsworthy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRG0603J10K </t>
   </si>
   <si>
     <t xml:space="preserve">C2,C1</t>
@@ -76,12 +76,6 @@
     <t xml:space="preserve">100nF</t>
   </si>
   <si>
-    <t xml:space="preserve">Vishay / Vitramon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VJ0603Y102JXAPW1BC </t>
-  </si>
-  <si>
     <t xml:space="preserve">R_CC2,R_CC1</t>
   </si>
   <si>
@@ -104,18 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">NXP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R_PROG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k Ohm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity / Holsworthy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRG0603J10K </t>
   </si>
   <si>
     <t xml:space="preserve">J_USB1</t>
@@ -211,7 +193,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,11 +206,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,6 +222,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -252,7 +336,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -263,7 +347,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,7 +366,7 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -308,7 +392,7 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -328,10 +412,10 @@
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -351,19 +435,15 @@
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -372,13 +452,13 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,76 +466,49 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>